<commit_message>
Prøver på ML. Har også oppdatert datasettet, det inneholder nå hele 2024!
</commit_message>
<xml_diff>
--- a/treningsdata.xlsx
+++ b/treningsdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="36">
   <si>
     <t>Dato</t>
   </si>
@@ -111,6 +111,15 @@
   <si>
     <t>Ahmed Abusaada</t>
   </si>
+  <si>
+    <t>Adrian Torvund</t>
+  </si>
+  <si>
+    <t>Erik Nordhagen</t>
+  </si>
+  <si>
+    <t>Johannes Aarra</t>
+  </si>
 </sst>
 </file>
 
@@ -143,12 +152,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -379,7 +391,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3671,6 +3683,2302 @@
       </c>
       <c r="D236" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1">
+        <v>2.0240706E7</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1">
+        <v>2.0240706E7</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1">
+        <v>2.0240706E7</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1">
+        <v>2.0240706E7</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1">
+        <v>2.0240706E7</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1">
+        <v>2.0240706E7</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1">
+        <v>2.0240706E7</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1">
+        <v>2.0240706E7</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1">
+        <v>2.0240706E7</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1">
+        <v>2.0240706E7</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1">
+        <v>2.0240715E7</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1">
+        <v>2.0240715E7</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1">
+        <v>2.0240715E7</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1">
+        <v>2.0240715E7</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1">
+        <v>2.0240715E7</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1">
+        <v>2.0240715E7</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1">
+        <v>2.0240715E7</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1">
+        <v>2.0240715E7</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1">
+        <v>2.0240722E7</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1">
+        <v>2.0240722E7</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1">
+        <v>2.0240722E7</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1">
+        <v>2.0240722E7</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1">
+        <v>2.0240722E7</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1">
+        <v>2.0240722E7</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1">
+        <v>2.0240722E7</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1">
+        <v>2.0240725E7</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1">
+        <v>2.0240725E7</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="1">
+        <v>2.0240725E7</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="1">
+        <v>2.0240725E7</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="1">
+        <v>2.0240725E7</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1">
+        <v>2.0240728E7</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D295" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="1">
+        <v>2.0240803E7</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D296" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D297" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D298" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D299" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D300" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D301" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D302" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D303" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D306" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D307" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D308" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D309" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D310" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1">
+        <v>2.024081E7</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D311" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D312" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D313" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D314" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D315" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D316" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D318" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D319" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D320" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D321" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="1">
+        <v>2.0240817E7</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D324" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="1">
+        <v>2.0240825E7</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D325" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="1">
+        <v>2.0240825E7</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="1">
+        <v>2.0240825E7</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D327" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="1">
+        <v>2.0240825E7</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D328" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="1">
+        <v>2.0240825E7</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D329" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="1">
+        <v>2.0240825E7</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D330" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1">
+        <v>2.0240825E7</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D331" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="1">
+        <v>2.0240825E7</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D332" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="1">
+        <v>2.0240825E7</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D333" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="1">
+        <v>2.0240825E7</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D334" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="1">
+        <v>2.0240825E7</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="1">
+        <v>2.0240825E7</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D336" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="1">
+        <v>2.0240831E7</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D337" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="1">
+        <v>2.0240831E7</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D338" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="1">
+        <v>2.0240831E7</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D339" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="1">
+        <v>2.0240831E7</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D340" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="1">
+        <v>2.0240831E7</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D341" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="1">
+        <v>2.0240831E7</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D342" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="1">
+        <v>2.0240831E7</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D343" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="1">
+        <v>2.0240831E7</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D344" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="1">
+        <v>2.0240831E7</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D345" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="1">
+        <v>2.0240831E7</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D346" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="1">
+        <v>2.0240831E7</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D347" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="1">
+        <v>2.0240831E7</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D348" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="1">
+        <v>2.0240908E7</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D349" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="1">
+        <v>2.0240908E7</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="1">
+        <v>2.0240908E7</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D351" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="1">
+        <v>2.0240908E7</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D352" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="1">
+        <v>2.0240908E7</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D353" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="1">
+        <v>2.0240908E7</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="1">
+        <v>2.0240908E7</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="1">
+        <v>2.0240908E7</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D356" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="1">
+        <v>2.0240908E7</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D357" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="1">
+        <v>2.0240908E7</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="1">
+        <v>2.0241002E7</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D359" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="1">
+        <v>2.0241002E7</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D360" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="1">
+        <v>2.0241002E7</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D361" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1">
+        <v>2.0241002E7</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="1">
+        <v>2.0241002E7</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1">
+        <v>2.0241008E7</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D364" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="1">
+        <v>2.0241008E7</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D365" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="1">
+        <v>2.0241008E7</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D366" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="1">
+        <v>2.0241008E7</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D367" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="1">
+        <v>2.0241008E7</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D368" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="1">
+        <v>2.0241008E7</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C369" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D369" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1">
+        <v>2.0241008E7</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D370" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1">
+        <v>2.0241008E7</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D371" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D372" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D373" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D374" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C375" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D375" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D376" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C377" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D377" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D378" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D379" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D380" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D381" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D382" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C383" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D383" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="1">
+        <v>2.024103E7</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C384" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D384" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="1">
+        <v>2.0241104E7</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C385" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D385" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="1">
+        <v>2.0241104E7</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D386" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="1">
+        <v>2.0241104E7</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C387" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D387" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="1">
+        <v>2.0241104E7</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C388" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D388" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="1">
+        <v>2.0241104E7</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D389" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="1">
+        <v>2.0241104E7</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D390" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="1">
+        <v>2.0241104E7</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D391" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="1">
+        <v>2.0241104E7</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D392" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="1">
+        <v>2.0241104E7</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C393" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D393" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="1">
+        <v>2.0241112E7</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D394" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="1">
+        <v>2.0241112E7</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D395" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="1">
+        <v>2.0241112E7</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D396" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="1">
+        <v>2.0241112E7</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C397" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D397" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="1">
+        <v>2.0241112E7</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C398" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D398" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="1">
+        <v>2.0241112E7</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C399" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D399" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="1">
+        <v>2.0241112E7</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C400" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D400" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Treningsdata består av 2025
</commit_message>
<xml_diff>
--- a/treningsdata.xlsx
+++ b/treningsdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="48">
   <si>
     <t>Dato</t>
   </si>
@@ -119,6 +119,42 @@
   </si>
   <si>
     <t>Johannes Aarra</t>
+  </si>
+  <si>
+    <t>Sami Bwoy IV</t>
+  </si>
+  <si>
+    <t>Rodas Breezy</t>
+  </si>
+  <si>
+    <t>Haakon Jordal</t>
+  </si>
+  <si>
+    <t>Henrik Haukefer Hauan</t>
+  </si>
+  <si>
+    <t>Anders Paulseth</t>
+  </si>
+  <si>
+    <t>Sondre Svendsen</t>
+  </si>
+  <si>
+    <t>Shewit Weldeslasie</t>
+  </si>
+  <si>
+    <t>Chewan Pokhrel</t>
+  </si>
+  <si>
+    <t>Jonas Tron Hatlem</t>
+  </si>
+  <si>
+    <t>Ionut Mititelu</t>
+  </si>
+  <si>
+    <t>Thomas Iyob</t>
+  </si>
+  <si>
+    <t>Maria Håland Alvik</t>
   </si>
 </sst>
 </file>
@@ -5981,6 +6017,3856 @@
         <v>5</v>
       </c>
     </row>
+    <row r="401">
+      <c r="A401" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C401" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D401" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D402" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C403" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D403" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C404" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D404" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B405" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C405" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D405" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C406" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D406" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C407" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D407" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D408" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C409" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D409" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C410" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D410" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D411" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B412" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C412" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D412" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B413" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C413" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D413" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D414" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B415" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D415" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D416" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="1">
+        <v>2.025012E7</v>
+      </c>
+      <c r="B417" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C417" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D417" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C418" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D418" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B419" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D419" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B420" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C420" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D420" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B421" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C421" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D421" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B422" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C422" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D422" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C423" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D423" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C424" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D424" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B425" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C425" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D425" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C426" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D426" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C427" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D427" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D428" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B429" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C429" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D429" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B430" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C430" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D430" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="1">
+        <v>2.0250126E7</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C431" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D431" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B432" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C432" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D432" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B433" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C433" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D433" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B434" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C434" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D434" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B435" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D435" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B436" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C436" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D436" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B437" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C437" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D437" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B438" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C438" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D438" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B439" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C439" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D439" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B440" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C440" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D440" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B441" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C441" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D441" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B442" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C442" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D442" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B443" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C443" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D443" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B444" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C444" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D444" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B445" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C445" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D445" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B446" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C446" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D446" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B447" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C447" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D447" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="1">
+        <v>2.0250203E7</v>
+      </c>
+      <c r="B448" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C448" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D448" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B449" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C449" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D449" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B450" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C450" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D450" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B451" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C451" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D451" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B452" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C452" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D452" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B453" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C453" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D453" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B454" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C454" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D454" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B455" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C455" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D455" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B456" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C456" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D456" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B457" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C457" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D457" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B458" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C458" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D458" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C459" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D459" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C460" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D460" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B461" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C461" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D461" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B462" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C462" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D462" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B463" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C463" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D463" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B464" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C464" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D464" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B465" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C465" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D465" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B466" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C466" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D466" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="1">
+        <v>2.0250209E7</v>
+      </c>
+      <c r="B467" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C467" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D467" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="1">
+        <v>2.0250218E7</v>
+      </c>
+      <c r="B468" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C468" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D468" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="1">
+        <v>2.0250218E7</v>
+      </c>
+      <c r="B469" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C469" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D469" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="1">
+        <v>2.0250218E7</v>
+      </c>
+      <c r="B470" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C470" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D470" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="1">
+        <v>2.0250218E7</v>
+      </c>
+      <c r="B471" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C471" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D471" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="1">
+        <v>2.0250218E7</v>
+      </c>
+      <c r="B472" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C472" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D472" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="1">
+        <v>2.0250218E7</v>
+      </c>
+      <c r="B473" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C473" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D473" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="1">
+        <v>2.0250218E7</v>
+      </c>
+      <c r="B474" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C474" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D474" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="1">
+        <v>2.0250218E7</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C475" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D475" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="1">
+        <v>2.0250218E7</v>
+      </c>
+      <c r="B476" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C476" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D476" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="1">
+        <v>2.0250218E7</v>
+      </c>
+      <c r="B477" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C477" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D477" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="1">
+        <v>2.0250218E7</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C478" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D478" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="1">
+        <v>2.0250218E7</v>
+      </c>
+      <c r="B479" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C479" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D479" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B480" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C480" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D480" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B481" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C481" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D481" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B482" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C482" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D482" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B483" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C483" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D483" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B484" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C484" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D484" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B485" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C485" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D485" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B486" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C486" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D486" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B487" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C487" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D487" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B488" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C488" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D488" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B489" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C489" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D489" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B490" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C490" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D490" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B491" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C491" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D491" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="1">
+        <v>2.0250223E7</v>
+      </c>
+      <c r="B492" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C492" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D492" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B493" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C493" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D493" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B494" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C494" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D494" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C495" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D495" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B496" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C496" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D496" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C497" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D497" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C498" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D498" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B499" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C499" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D499" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C500" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D500" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C501" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D501" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C502" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D502" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C503" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D503" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C504" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D504" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C505" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D505" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C506" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D506" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C507" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D507" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="1">
+        <v>2.0250302E7</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C508" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D508" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C509" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D509" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C510" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D510" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C511" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D511" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C512" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D512" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C513" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D513" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C514" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D514" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B515" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C515" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D515" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C516" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D516" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C517" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D517" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C518" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D518" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C519" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D519" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C520" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D520" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C521" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D521" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C522" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D522" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C523" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D523" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B524" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C524" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D524" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B525" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C525" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D525" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B526" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C526" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D526" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" s="1">
+        <v>2.025031E7</v>
+      </c>
+      <c r="B527" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C527" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D527" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" s="1">
+        <v>2.0250316E7</v>
+      </c>
+      <c r="B528" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C528" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D528" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" s="1">
+        <v>2.0250316E7</v>
+      </c>
+      <c r="B529" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C529" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D529" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="1">
+        <v>2.0250316E7</v>
+      </c>
+      <c r="B530" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C530" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D530" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" s="1">
+        <v>2.0250316E7</v>
+      </c>
+      <c r="B531" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C531" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D531" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="1">
+        <v>2.0250316E7</v>
+      </c>
+      <c r="B532" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C532" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D532" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="1">
+        <v>2.0250316E7</v>
+      </c>
+      <c r="B533" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C533" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D533" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="1">
+        <v>2.0250316E7</v>
+      </c>
+      <c r="B534" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C534" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D534" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" s="1">
+        <v>2.0250316E7</v>
+      </c>
+      <c r="B535" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C535" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D535" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="1">
+        <v>2.0250316E7</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C536" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D536" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="1">
+        <v>2.0250316E7</v>
+      </c>
+      <c r="B537" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C537" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D537" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="1">
+        <v>2.0250316E7</v>
+      </c>
+      <c r="B538" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C538" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D538" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B539" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C539" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D539" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B540" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C540" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D540" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B541" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C541" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D541" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B542" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C542" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D542" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B543" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C543" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D543" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B544" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C544" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D544" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B545" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C545" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D545" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B546" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C546" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D546" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B547" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C547" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D547" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B548" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C548" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D548" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B549" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C549" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D549" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B550" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C550" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D550" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B551" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C551" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D551" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B552" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C552" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D552" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B553" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C553" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D553" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B554" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C554" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D554" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B555" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C555" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D555" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="1">
+        <v>2.0250323E7</v>
+      </c>
+      <c r="B556" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C556" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D556" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C557" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D557" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C558" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D558" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C559" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D559" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C560" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D560" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B561" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C561" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D561" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B562" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C562" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D562" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C563" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D563" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C564" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D564" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C565" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D565" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C566" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D566" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B567" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C567" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D567" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B568" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C568" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D568" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B569" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C569" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D569" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B570" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C570" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D570" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B571" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C571" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D571" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" s="1">
+        <v>2.025033E7</v>
+      </c>
+      <c r="B572" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C572" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D572" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B573" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C573" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D573" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B574" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C574" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D574" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B575" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C575" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D575" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B576" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C576" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D576" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B577" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C577" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D577" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B578" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C578" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D578" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B579" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C579" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D579" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B580" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C580" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D580" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B581" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C581" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D581" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B582" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C582" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D582" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B583" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C583" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D583" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B584" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C584" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D584" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B585" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C585" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D585" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B586" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C586" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D586" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B587" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C587" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D587" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B588" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C588" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D588" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B589" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C589" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D589" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" s="1">
+        <v>2.0250406E7</v>
+      </c>
+      <c r="B590" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C590" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D590" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B591" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C591" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D591" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B592" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C592" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D592" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B593" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C593" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D593" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B594" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C594" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D594" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B595" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C595" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D595" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B596" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C596" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D596" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B597" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C597" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D597" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B598" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C598" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D598" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B599" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C599" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D599" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B600" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C600" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D600" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B601" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C601" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D601" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B602" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C602" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D602" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B603" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C603" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D603" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B604" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C604" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D604" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" s="1">
+        <v>2.0250413E7</v>
+      </c>
+      <c r="B605" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C605" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D605" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B606" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C606" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D606" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B607" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C607" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D607" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B608" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C608" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D608" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B609" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C609" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D609" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B610" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C610" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D610" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B611" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C611" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D611" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B612" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C612" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D612" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B613" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C613" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D613" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B614" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C614" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D614" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B615" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C615" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D615" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B616" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C616" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D616" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B617" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C617" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D617" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B618" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C618" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D618" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" s="1">
+        <v>2.025042E7</v>
+      </c>
+      <c r="B619" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C619" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D619" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B620" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C620" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D620" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B621" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C621" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D621" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B622" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C622" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D622" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B623" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C623" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D623" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B624" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C624" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D624" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B625" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C625" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D625" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B626" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C626" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D626" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B627" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C627" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D627" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B628" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C628" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D628" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B629" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C629" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D629" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B630" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C630" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D630" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B631" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C631" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D631" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B632" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C632" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D632" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B633" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C633" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D633" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" s="1">
+        <v>2.0250427E7</v>
+      </c>
+      <c r="B634" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C634" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D634" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B635" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C635" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D635" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B636" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C636" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D636" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B637" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C637" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D637" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B638" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C638" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D638" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B639" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C639" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D639" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B640" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C640" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D640" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B641" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C641" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D641" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B642" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C642" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D642" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B643" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C643" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D643" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B644" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C644" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D644" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B645" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C645" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D645" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B646" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C646" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D646" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B647" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C647" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D647" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B648" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C648" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D648" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" s="1">
+        <v>2.0250504E7</v>
+      </c>
+      <c r="B649" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C649" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D649" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B650" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C650" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D650" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B651" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C651" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D651" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B652" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C652" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D652" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B653" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C653" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D653" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B654" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C654" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D654" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B655" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C655" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D655" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B656" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C656" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D656" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B657" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C657" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D657" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B658" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C658" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D658" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B659" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C659" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D659" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B660" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C660" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D660" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B661" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C661" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D661" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B662" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C662" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D662" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B663" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C663" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D663" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B664" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C664" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D664" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" s="1">
+        <v>2.0250511E7</v>
+      </c>
+      <c r="B665" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C665" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D665" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" s="1">
+        <v>2.0250518E7</v>
+      </c>
+      <c r="B666" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C666" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D666" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" s="1">
+        <v>2.0250518E7</v>
+      </c>
+      <c r="B667" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C667" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D667" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" s="1">
+        <v>2.0250518E7</v>
+      </c>
+      <c r="B668" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C668" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D668" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" s="1">
+        <v>2.0250518E7</v>
+      </c>
+      <c r="B669" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C669" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D669" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" s="1">
+        <v>2.0250518E7</v>
+      </c>
+      <c r="B670" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C670" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D670" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" s="1">
+        <v>2.0250518E7</v>
+      </c>
+      <c r="B671" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C671" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D671" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" s="1">
+        <v>2.0250518E7</v>
+      </c>
+      <c r="B672" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C672" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D672" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" s="1">
+        <v>2.0250518E7</v>
+      </c>
+      <c r="B673" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C673" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D673" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" s="1">
+        <v>2.0250518E7</v>
+      </c>
+      <c r="B674" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C674" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D674" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" s="1">
+        <v>2.0250518E7</v>
+      </c>
+      <c r="B675" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C675" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D675" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Oppdatert en feil i datasettet, samt skrevet logikk for å finne første mandagen eller onsdagen etter publiseringsdato
</commit_message>
<xml_diff>
--- a/treningsdata.xlsx
+++ b/treningsdata.xlsx
@@ -5613,7 +5613,7 @@
     </row>
     <row r="372">
       <c r="A372" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B372" s="1" t="s">
         <v>6</v>
@@ -5627,7 +5627,7 @@
     </row>
     <row r="373">
       <c r="A373" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B373" s="1" t="s">
         <v>12</v>
@@ -5641,7 +5641,7 @@
     </row>
     <row r="374">
       <c r="A374" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B374" s="1" t="s">
         <v>21</v>
@@ -5655,7 +5655,7 @@
     </row>
     <row r="375">
       <c r="A375" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B375" s="1" t="s">
         <v>16</v>
@@ -5669,7 +5669,7 @@
     </row>
     <row r="376">
       <c r="A376" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B376" s="1" t="s">
         <v>8</v>
@@ -5683,7 +5683,7 @@
     </row>
     <row r="377">
       <c r="A377" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B377" s="1" t="s">
         <v>18</v>
@@ -5697,7 +5697,7 @@
     </row>
     <row r="378">
       <c r="A378" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B378" s="1" t="s">
         <v>10</v>
@@ -5711,7 +5711,7 @@
     </row>
     <row r="379">
       <c r="A379" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B379" s="1" t="s">
         <v>19</v>
@@ -5725,7 +5725,7 @@
     </row>
     <row r="380">
       <c r="A380" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B380" s="1" t="s">
         <v>24</v>
@@ -5739,7 +5739,7 @@
     </row>
     <row r="381">
       <c r="A381" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B381" s="1" t="s">
         <v>7</v>
@@ -5753,7 +5753,7 @@
     </row>
     <row r="382">
       <c r="A382" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B382" s="1" t="s">
         <v>13</v>
@@ -5767,7 +5767,7 @@
     </row>
     <row r="383">
       <c r="A383" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B383" s="1" t="s">
         <v>35</v>
@@ -5781,7 +5781,7 @@
     </row>
     <row r="384">
       <c r="A384" s="1">
-        <v>2.024103E7</v>
+        <v>2.0241028E7</v>
       </c>
       <c r="B384" s="1" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Oppdatert trenignsdata og lagt inn ny versjon av polars
</commit_message>
<xml_diff>
--- a/treningsdata.xlsx
+++ b/treningsdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3370" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3415" uniqueCount="58">
   <si>
     <t>Dato</t>
   </si>
@@ -16170,49 +16170,214 @@
       </c>
     </row>
     <row r="1124">
-      <c r="B1124" s="1"/>
+      <c r="A1124" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1124" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1124" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1124" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1125">
-      <c r="B1125" s="1"/>
+      <c r="A1125" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1125" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1125" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1125" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1126">
-      <c r="B1126" s="1"/>
+      <c r="A1126" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1126" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1126" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1126" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1127">
-      <c r="B1127" s="1"/>
+      <c r="A1127" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1127" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1127" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1127" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1128">
-      <c r="B1128" s="1"/>
+      <c r="A1128" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1128" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1128" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1128" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1129">
-      <c r="B1129" s="1"/>
+      <c r="A1129" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1129" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1129" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1129" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1130">
-      <c r="B1130" s="1"/>
+      <c r="A1130" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1130" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1130" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1130" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1131">
-      <c r="B1131" s="1"/>
+      <c r="A1131" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1131" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1131" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1131" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1132">
-      <c r="B1132" s="1"/>
+      <c r="A1132" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1132" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1132" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1132" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1133">
-      <c r="B1133" s="1"/>
+      <c r="A1133" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1133" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1133" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1133" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1134">
-      <c r="B1134" s="1"/>
+      <c r="A1134" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1134" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1134" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1134" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1135">
-      <c r="B1135" s="1"/>
+      <c r="A1135" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1135" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1135" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1135" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1136">
-      <c r="B1136" s="1"/>
+      <c r="A1136" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1136" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1136" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1136" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1137">
-      <c r="B1137" s="1"/>
+      <c r="A1137" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1137" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1137" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1137" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1138">
-      <c r="B1138" s="1"/>
+      <c r="A1138" s="1">
+        <v>2.0251227E7</v>
+      </c>
+      <c r="B1138" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1138" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1138" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="1139">
       <c r="B1139" s="1"/>

</xml_diff>